<commit_message>
modified:   Brighway/Results/Ananas sub - CONSQ.xlsx 	modified:   Brighway/Rune BE.ipynb 	modified:   Brighway/monte_carlo_simulations_Rune.xlsx
</commit_message>
<xml_diff>
--- a/Brighway/monte_carlo_simulations_Rune.xlsx
+++ b/Brighway/monte_carlo_simulations_Rune.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruw\Desktop\RA\Single-use-vs-multi-use-in-health-care\Brighway\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA1993B-7AB3-4374-985D-9364CAF94DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="acidification" sheetId="1" r:id="rId1"/>
@@ -30,7 +24,7 @@
     <sheet name="photochemical oxidant formation" sheetId="15" r:id="rId15"/>
     <sheet name="water use" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -64,8 +58,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,24 +121,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{37CACE69-0D20-434D-BAB8-AB4441BA8BA2}"/>
-  </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -182,7 +166,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -216,7 +200,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -251,10 +234,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,14 +409,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,74 +427,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1.2712286684667919E-2</v>
+        <v>0.01301890860565253</v>
       </c>
       <c r="C2">
-        <v>6.890720884323312E-2</v>
+        <v>0.04492728020958839</v>
       </c>
       <c r="D2">
-        <v>0.1281306409217578</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.09396305350820852</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1.2712286684667919E-2</v>
+        <v>0.01301890860565253</v>
       </c>
       <c r="C3">
-        <v>6.890720884323312E-2</v>
+        <v>0.04492728020958839</v>
       </c>
       <c r="D3">
-        <v>0.1281306409217578</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.09396305350820852</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2.9532593968229539E-4</v>
+        <v>5.570424818366303E-05</v>
       </c>
       <c r="C4">
-        <v>2.5657464480004291E-3</v>
+        <v>0.0002744590413067162</v>
       </c>
       <c r="D4">
-        <v>7.4225665843680039E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.001632990653516388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1.241696074498563E-2</v>
+        <v>0.01296320435746887</v>
       </c>
       <c r="C5">
-        <v>6.6341462395232698E-2</v>
+        <v>0.04465282116828167</v>
       </c>
       <c r="D5">
-        <v>0.1207080743373898</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.09233006285469214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>1.3007612624350221E-2</v>
+        <v>0.0130746128538362</v>
       </c>
       <c r="C6">
-        <v>7.1472955291233556E-2</v>
+        <v>0.0452017392508951</v>
       </c>
       <c r="D6">
-        <v>0.13555320750612579</v>
+        <v>0.09559604416172492</v>
       </c>
     </row>
   </sheetData>
@@ -521,14 +503,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,74 +521,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.48082193871665202</v>
+        <v>0.4743081605562167</v>
       </c>
       <c r="C2">
-        <v>0.53265021181075589</v>
+        <v>0.4994842091335284</v>
       </c>
       <c r="D2">
-        <v>0.57594238991971403</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.5255423270207827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.48082193871665202</v>
+        <v>0.4743081605562167</v>
       </c>
       <c r="C3">
-        <v>0.53265021181075589</v>
+        <v>0.4994842091335284</v>
       </c>
       <c r="D3">
-        <v>0.57594238991971403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.5255423270207827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>9.6536659297949412E-3</v>
+        <v>0.008345112578410724</v>
       </c>
       <c r="C4">
-        <v>9.1607752642052231E-3</v>
+        <v>0.005973731135541116</v>
       </c>
       <c r="D4">
-        <v>1.008558089321587E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.008235561142397541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.47116827278685702</v>
+        <v>0.465963047977806</v>
       </c>
       <c r="C5">
-        <v>0.52348943654655067</v>
+        <v>0.4935104779979873</v>
       </c>
       <c r="D5">
-        <v>0.56585680902649815</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.5173067658783852</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.49047560464644691</v>
+        <v>0.4826532731346274</v>
       </c>
       <c r="C6">
-        <v>0.54181098707496111</v>
+        <v>0.5054579402690695</v>
       </c>
       <c r="D6">
-        <v>0.5860279708129299</v>
+        <v>0.5337778881631803</v>
       </c>
     </row>
   </sheetData>
@@ -615,14 +597,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,74 +615,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>33.749005075123847</v>
+        <v>33.22579509436196</v>
       </c>
       <c r="C2">
-        <v>124.1914537309373</v>
+        <v>122.7236790476476</v>
       </c>
       <c r="D2">
-        <v>72.992204701632801</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69.21073123572077</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>33.749005075123847</v>
+        <v>33.22579509436196</v>
       </c>
       <c r="C3">
-        <v>124.1914537309373</v>
+        <v>122.7236790476476</v>
       </c>
       <c r="D3">
-        <v>72.992204701632801</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69.21073123572077</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.84336732471166798</v>
+        <v>0.2397223712882877</v>
       </c>
       <c r="C4">
-        <v>14.76651158055213</v>
+        <v>2.83080562140357</v>
       </c>
       <c r="D4">
-        <v>5.886775100651775</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.555176117098803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>32.905637750412183</v>
+        <v>32.98607272307368</v>
       </c>
       <c r="C5">
-        <v>109.42494215038511</v>
+        <v>119.892873426244</v>
       </c>
       <c r="D5">
-        <v>67.105429600981026</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64.65555511862196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>34.592372399835511</v>
+        <v>33.46551746565025</v>
       </c>
       <c r="C6">
-        <v>138.9579653114894</v>
+        <v>125.5544846690511</v>
       </c>
       <c r="D6">
-        <v>78.878979802284576</v>
+        <v>73.76590735281957</v>
       </c>
     </row>
   </sheetData>
@@ -709,14 +691,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,74 +709,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4.0665772701128638E-5</v>
+        <v>4.070350128012493E-05</v>
       </c>
       <c r="C2">
-        <v>1.062797298894402E-4</v>
+        <v>9.094841088417582E-05</v>
       </c>
       <c r="D2">
-        <v>1.6806960467194421E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0001139361547805559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>4.0665772701128638E-5</v>
+        <v>4.070350128012493E-05</v>
       </c>
       <c r="C3">
-        <v>1.062797298894402E-4</v>
+        <v>9.094841088417582E-05</v>
       </c>
       <c r="D3">
-        <v>1.6806960467194421E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0001139361547805559</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>9.4537174746326221E-7</v>
+        <v>1.154671259574353E-06</v>
       </c>
       <c r="C4">
-        <v>6.4767671411802009E-6</v>
+        <v>4.601916185485692E-07</v>
       </c>
       <c r="D4">
-        <v>3.8594613803250363E-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7.99303836054593E-07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3.9720400953665383E-5</v>
+        <v>3.954883002055058E-05</v>
       </c>
       <c r="C5">
-        <v>9.9802962748259957E-5</v>
+        <v>9.048821926562724E-05</v>
       </c>
       <c r="D5">
-        <v>1.6421014329161921E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0001131368509445013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>4.1611144448591901E-5</v>
+        <v>4.185817253969928E-05</v>
       </c>
       <c r="C6">
-        <v>1.127564970306204E-4</v>
+        <v>9.140860250272438E-05</v>
       </c>
       <c r="D6">
-        <v>1.7192906605226931E-4</v>
+        <v>0.0001147354586166105</v>
       </c>
     </row>
   </sheetData>
@@ -803,14 +785,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,74 +803,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1.9709827860354799E-7</v>
+        <v>1.689073654350229E-07</v>
       </c>
       <c r="C2">
-        <v>2.4482503242001498E-7</v>
+        <v>2.148907417388324E-07</v>
       </c>
       <c r="D2">
-        <v>2.601476872327198E-7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.239018499883693E-07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1.9709827860354799E-7</v>
+        <v>1.689073654350229E-07</v>
       </c>
       <c r="C3">
-        <v>2.4482503242001498E-7</v>
+        <v>2.148907417388324E-07</v>
       </c>
       <c r="D3">
-        <v>2.601476872327198E-7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.239018499883693E-07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1.928906384686035E-8</v>
+        <v>1.834321240362169E-08</v>
       </c>
       <c r="C4">
-        <v>1.7753292075093829E-8</v>
+        <v>1.816513653252737E-08</v>
       </c>
       <c r="D4">
-        <v>1.7511578941107189E-8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.043228481913988E-08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1.778092147566876E-7</v>
+        <v>1.505641530314012E-07</v>
       </c>
       <c r="C5">
-        <v>2.2707174034492121E-7</v>
+        <v>1.96725605206305E-07</v>
       </c>
       <c r="D5">
-        <v>2.4263610829161261E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.134695651692294E-07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2.163873424504083E-7</v>
+        <v>1.872505778386446E-07</v>
       </c>
       <c r="C6">
-        <v>2.6257832449510878E-7</v>
+        <v>2.330558782713597E-07</v>
       </c>
       <c r="D6">
-        <v>2.7765926617382699E-7</v>
+        <v>2.343341348075092E-07</v>
       </c>
     </row>
   </sheetData>
@@ -897,14 +879,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,74 +897,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>7.7101009606068038E-8</v>
+        <v>7.153251759324002E-08</v>
       </c>
       <c r="C2">
-        <v>1.6705933182225371E-7</v>
+        <v>1.484018248613936E-07</v>
       </c>
       <c r="D2">
-        <v>1.9784436417848329E-7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.447548950878582E-07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>7.7101009606068038E-8</v>
+        <v>7.153251759324002E-08</v>
       </c>
       <c r="C3">
-        <v>1.6705933182225371E-7</v>
+        <v>1.484018248613936E-07</v>
       </c>
       <c r="D3">
-        <v>1.9784436417848329E-7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.447548950878582E-07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2.9836037272561342E-9</v>
+        <v>1.776562980428456E-09</v>
       </c>
       <c r="C4">
-        <v>1.045722485619781E-8</v>
+        <v>3.236489267969822E-09</v>
       </c>
       <c r="D4">
-        <v>9.6804772244753392E-9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.074552547196286E-08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>7.4117405878811904E-8</v>
+        <v>6.975595461281157E-08</v>
       </c>
       <c r="C5">
-        <v>1.566021069660558E-7</v>
+        <v>1.451653355934238E-07</v>
       </c>
       <c r="D5">
-        <v>1.8816388695400789E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.340093696158953E-07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>8.0084613333324172E-8</v>
+        <v>7.330908057366848E-08</v>
       </c>
       <c r="C6">
-        <v>1.7751655667845149E-7</v>
+        <v>1.516383141293634E-07</v>
       </c>
       <c r="D6">
-        <v>2.0752484140295859E-7</v>
+        <v>1.555004205598211E-07</v>
       </c>
     </row>
   </sheetData>
@@ -991,14 +973,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,74 +991,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>8.4523877804438749E-3</v>
+        <v>0.008198499539162515</v>
       </c>
       <c r="C2">
-        <v>1.5412785038615611E-2</v>
+        <v>0.01320115763433961</v>
       </c>
       <c r="D2">
-        <v>1.8877420369027249E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.01704941302474294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>8.4523877804438749E-3</v>
+        <v>0.008198499539162515</v>
       </c>
       <c r="C3">
-        <v>1.5412785038615611E-2</v>
+        <v>0.01320115763433961</v>
       </c>
       <c r="D3">
-        <v>1.8877420369027249E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.01704941302474294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2.350068071800878E-4</v>
+        <v>9.582588056965442E-05</v>
       </c>
       <c r="C4">
-        <v>7.1415689840930927E-4</v>
+        <v>0.001120594408849505</v>
       </c>
       <c r="D4">
-        <v>7.0841814546558808E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.002540908138188803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>8.2173809732637871E-3</v>
+        <v>0.00810267365859286</v>
       </c>
       <c r="C5">
-        <v>1.46986281402063E-2</v>
+        <v>0.0120805632254901</v>
       </c>
       <c r="D5">
-        <v>1.8169002223561659E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.01450850488655414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>8.6873945876239627E-3</v>
+        <v>0.008294325419732169</v>
       </c>
       <c r="C6">
-        <v>1.6126941937024918E-2</v>
+        <v>0.01432175204318911</v>
       </c>
       <c r="D6">
-        <v>1.9585838514492832E-2</v>
+        <v>0.01959032116293174</v>
       </c>
     </row>
   </sheetData>
@@ -1085,14 +1067,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1103,74 +1085,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4.9356171362608041</v>
+        <v>4.945474181071563</v>
       </c>
       <c r="C2">
-        <v>5.2285205960568852</v>
+        <v>5.072200063319665</v>
       </c>
       <c r="D2">
-        <v>5.3021491334103219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.132090208043695</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>4.9356171362608041</v>
+        <v>4.945474181071563</v>
       </c>
       <c r="C3">
-        <v>5.2285205960568852</v>
+        <v>5.072200063319665</v>
       </c>
       <c r="D3">
-        <v>5.3021491334103219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.132090208043695</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>8.6917005165493055E-2</v>
+        <v>0.2438396840777006</v>
       </c>
       <c r="C4">
-        <v>8.9459449162176075E-2</v>
+        <v>0.228101202100643</v>
       </c>
       <c r="D4">
-        <v>8.6391204125651377E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.1155501885131782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>4.8487001310953106</v>
+        <v>4.701634496993862</v>
       </c>
       <c r="C5">
-        <v>5.1390611468947087</v>
+        <v>4.844098861219021</v>
       </c>
       <c r="D5">
-        <v>5.2157579292846714</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.016540019530517</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>5.0225341414262967</v>
+        <v>5.189313865149264</v>
       </c>
       <c r="C6">
-        <v>5.3179800452190609</v>
+        <v>5.300301265420307</v>
       </c>
       <c r="D6">
-        <v>5.3885403375359733</v>
+        <v>5.247640396556873</v>
       </c>
     </row>
   </sheetData>
@@ -1179,14 +1161,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1197,74 +1179,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>611.24794386559188</v>
+        <v>685.91515672819</v>
       </c>
       <c r="C2">
-        <v>130.5034023578352</v>
+        <v>121.8478955855811</v>
       </c>
       <c r="D2">
-        <v>130.72111541177421</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>154.3014603481306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>611.24794386559188</v>
+        <v>685.91515672819</v>
       </c>
       <c r="C3">
-        <v>130.5034023578352</v>
+        <v>121.8478955855811</v>
       </c>
       <c r="D3">
-        <v>130.72111541177421</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>154.3014603481306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>73.031728446461216</v>
+        <v>34.1650299939123</v>
       </c>
       <c r="C4">
-        <v>20.480635423103539</v>
+        <v>7.854681090856801</v>
       </c>
       <c r="D4">
-        <v>20.46223692235662</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39.05851847948421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>538.21621541913066</v>
+        <v>651.7501267342777</v>
       </c>
       <c r="C5">
-        <v>110.02276693473171</v>
+        <v>113.9932144947243</v>
       </c>
       <c r="D5">
-        <v>110.2588784894176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115.2429418686464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>684.27967231205309</v>
+        <v>720.0801867221023</v>
       </c>
       <c r="C6">
-        <v>150.98403778093871</v>
+        <v>129.7025766764379</v>
       </c>
       <c r="D6">
-        <v>151.1833523341308</v>
+        <v>193.3599788276148</v>
       </c>
     </row>
   </sheetData>
@@ -1273,14 +1255,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1291,74 +1273,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>18.456260800132871</v>
+        <v>18.46188626739342</v>
       </c>
       <c r="C2">
-        <v>23.59725795623746</v>
+        <v>21.92044833494302</v>
       </c>
       <c r="D2">
-        <v>28.2440587508414</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24.5703240585126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>18.456260800132871</v>
+        <v>18.46188626739342</v>
       </c>
       <c r="C3">
-        <v>23.59725795623746</v>
+        <v>21.92044833494302</v>
       </c>
       <c r="D3">
-        <v>28.2440587508414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24.5703240585126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.48087489237149939</v>
+        <v>0.3781569221883387</v>
       </c>
       <c r="C4">
-        <v>0.79737594959133595</v>
+        <v>0.3910035400873237</v>
       </c>
       <c r="D4">
-        <v>0.61055285401993586</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.7025926479857443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>17.975385907761371</v>
+        <v>18.08372934520508</v>
       </c>
       <c r="C5">
-        <v>22.799882006646129</v>
+        <v>21.5294447948557</v>
       </c>
       <c r="D5">
-        <v>27.633505896821461</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23.86773141052686</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>18.93713569250437</v>
+        <v>18.84004318958176</v>
       </c>
       <c r="C6">
-        <v>24.394633905828801</v>
+        <v>22.31145187503034</v>
       </c>
       <c r="D6">
-        <v>28.85461160486134</v>
+        <v>25.27291670649835</v>
       </c>
     </row>
   </sheetData>
@@ -1367,14 +1349,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,74 +1367,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>53.852073249494843</v>
+        <v>54.27614752317398</v>
       </c>
       <c r="C2">
-        <v>61.057945143713702</v>
+        <v>57.19583025550671</v>
       </c>
       <c r="D2">
-        <v>64.975767306229116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59.89841754229741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>53.852073249494843</v>
+        <v>54.27614752317398</v>
       </c>
       <c r="C3">
-        <v>61.057945143713702</v>
+        <v>57.19583025550671</v>
       </c>
       <c r="D3">
-        <v>64.975767306229116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59.89841754229741</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1.287383108449667</v>
+        <v>0.2737799150218905</v>
       </c>
       <c r="C4">
-        <v>1.4853376619821359</v>
+        <v>0.9598599338312575</v>
       </c>
       <c r="D4">
-        <v>1.3499687467575081</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.731748018272874</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>52.564690141045169</v>
+        <v>54.00236760815209</v>
       </c>
       <c r="C5">
-        <v>59.572607481731559</v>
+        <v>56.23597032167545</v>
       </c>
       <c r="D5">
-        <v>63.625798559471612</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56.16666952402453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>55.139456357944503</v>
+        <v>54.54992743819587</v>
       </c>
       <c r="C6">
-        <v>62.543282805695831</v>
+        <v>58.15569018933796</v>
       </c>
       <c r="D6">
-        <v>66.325736052986628</v>
+        <v>63.63016556057028</v>
       </c>
     </row>
   </sheetData>
@@ -1461,14 +1443,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1479,74 +1461,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1.0552791742957049E-3</v>
+        <v>0.001052382898561331</v>
       </c>
       <c r="C2">
-        <v>1.336571104320914E-3</v>
+        <v>0.001274974337902841</v>
       </c>
       <c r="D2">
-        <v>1.6575828567555221E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.001469227668541239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1.0552791742957049E-3</v>
+        <v>0.001052382898561331</v>
       </c>
       <c r="C3">
-        <v>1.336571104320914E-3</v>
+        <v>0.001274974337902841</v>
       </c>
       <c r="D3">
-        <v>1.6575828567555221E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.001469227668541239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2.2887854061216469E-5</v>
+        <v>3.567192616413034E-05</v>
       </c>
       <c r="C4">
-        <v>3.5761587259199967E-5</v>
+        <v>1.217575818474763E-05</v>
       </c>
       <c r="D4">
-        <v>2.7353145114355351E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.562253759366682E-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1.0323913202344879E-3</v>
+        <v>0.001016710972397201</v>
       </c>
       <c r="C5">
-        <v>1.300809517061714E-3</v>
+        <v>0.001262798579718093</v>
       </c>
       <c r="D5">
-        <v>1.630229711641167E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.001453605130947572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>1.0781670283569211E-3</v>
+        <v>0.001088054824725462</v>
       </c>
       <c r="C6">
-        <v>1.3723326915801139E-3</v>
+        <v>0.001287150096087588</v>
       </c>
       <c r="D6">
-        <v>1.684936001869877E-3</v>
+        <v>0.001484850206134906</v>
       </c>
     </row>
   </sheetData>
@@ -1555,14 +1537,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1573,74 +1555,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5.9389217508267938E-3</v>
+        <v>0.005785842738884175</v>
       </c>
       <c r="C2">
-        <v>7.122717713226057E-3</v>
+        <v>0.006733317976327258</v>
       </c>
       <c r="D2">
-        <v>6.9165507570479656E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.006429981047488167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>5.9389217508267938E-3</v>
+        <v>0.005785842738884175</v>
       </c>
       <c r="C3">
-        <v>7.122717713226057E-3</v>
+        <v>0.006733317976327258</v>
       </c>
       <c r="D3">
-        <v>6.9165507570479656E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.006429981047488167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1.210140610578029E-4</v>
+        <v>0.0001764611905318838</v>
       </c>
       <c r="C4">
-        <v>2.3379131507041001E-4</v>
+        <v>0.0001392066491275952</v>
       </c>
       <c r="D4">
-        <v>1.272643367878686E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0002275792162166413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>5.8179076897689908E-3</v>
+        <v>0.005609381548352291</v>
       </c>
       <c r="C5">
-        <v>6.8889263981556474E-3</v>
+        <v>0.006594111327199662</v>
       </c>
       <c r="D5">
-        <v>6.7892864202600978E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.006202401831271525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>6.0599358118845967E-3</v>
+        <v>0.005962303929416058</v>
       </c>
       <c r="C6">
-        <v>7.3565090282964674E-3</v>
+        <v>0.006872524625454852</v>
       </c>
       <c r="D6">
-        <v>7.0438150938358351E-3</v>
+        <v>0.006657560263704808</v>
       </c>
     </row>
   </sheetData>
@@ -1649,14 +1631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1667,74 +1649,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3.4479977789054587E-2</v>
+        <v>0.03348745466523952</v>
       </c>
       <c r="C2">
-        <v>5.0146371206153062E-2</v>
+        <v>0.04997865173765363</v>
       </c>
       <c r="D2">
-        <v>4.5113888169428989E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.04208065970262347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>3.4479977789054587E-2</v>
+        <v>0.03348745466523952</v>
       </c>
       <c r="C3">
-        <v>5.0146371206153062E-2</v>
+        <v>0.04997865173765363</v>
       </c>
       <c r="D3">
-        <v>4.5113888169428989E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.04208065970262347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>7.7895013904492189E-4</v>
+        <v>0.0003945522394285701</v>
       </c>
       <c r="C4">
-        <v>2.6709514027387009E-3</v>
+        <v>0.0005667728119555238</v>
       </c>
       <c r="D4">
-        <v>1.00693900978676E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0003346920328141795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3.3701027650009673E-2</v>
+        <v>0.03309290242581095</v>
       </c>
       <c r="C5">
-        <v>4.7475419803414361E-2</v>
+        <v>0.04941187892569811</v>
       </c>
       <c r="D5">
-        <v>4.4106949159642229E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.04174596766980929</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>3.5258927928099509E-2</v>
+        <v>0.03388200690466809</v>
       </c>
       <c r="C6">
-        <v>5.2817322608891763E-2</v>
+        <v>0.05054542454960916</v>
       </c>
       <c r="D6">
-        <v>4.612082717921575E-2</v>
+        <v>0.04241535173543765</v>
       </c>
     </row>
   </sheetData>
@@ -1743,14 +1725,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1761,74 +1743,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1.774299163884973E-9</v>
+        <v>1.737408483354102E-09</v>
       </c>
       <c r="C2">
-        <v>3.173420243801626E-9</v>
+        <v>2.979426341356907E-09</v>
       </c>
       <c r="D2">
-        <v>3.6284923073394359E-9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.109563011398316E-09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1.774299163884973E-9</v>
+        <v>1.737408483354102E-09</v>
       </c>
       <c r="C3">
-        <v>3.173420243801626E-9</v>
+        <v>2.979426341356907E-09</v>
       </c>
       <c r="D3">
-        <v>3.6284923073394359E-9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.109563011398316E-09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>4.7899729817781362E-11</v>
+        <v>1.323561218925593E-10</v>
       </c>
       <c r="C4">
-        <v>1.978121403506154E-10</v>
+        <v>1.86439588265648E-10</v>
       </c>
       <c r="D4">
-        <v>7.1259727465954793E-11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.810144995937734E-10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1.726399434067192E-9</v>
+        <v>1.605052361461542E-09</v>
       </c>
       <c r="C5">
-        <v>2.9756081034510112E-9</v>
+        <v>2.792986753091259E-09</v>
       </c>
       <c r="D5">
-        <v>3.5572325798734819E-9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.928548511804542E-09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>1.8221988937027541E-9</v>
+        <v>1.869764605246661E-09</v>
       </c>
       <c r="C6">
-        <v>3.371232384152242E-9</v>
+        <v>3.165865929622555E-09</v>
       </c>
       <c r="D6">
-        <v>3.6997520348053911E-9</v>
+        <v>3.290577510992089E-09</v>
       </c>
     </row>
   </sheetData>
@@ -1837,14 +1819,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1855,74 +1837,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>6.8399854140173077E-8</v>
+        <v>6.706026327272075E-08</v>
       </c>
       <c r="C2">
-        <v>7.2750582984433794E-8</v>
+        <v>6.186889874267598E-08</v>
       </c>
       <c r="D2">
-        <v>6.2772995074764035E-8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.611203604327117E-08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>6.8399854140173077E-8</v>
+        <v>6.706026327272075E-08</v>
       </c>
       <c r="C3">
-        <v>7.2750582984433794E-8</v>
+        <v>6.186889874267598E-08</v>
       </c>
       <c r="D3">
-        <v>6.2772995074764035E-8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.611203604327117E-08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>5.2138472000542768E-9</v>
+        <v>4.222551249701617E-09</v>
       </c>
       <c r="C4">
-        <v>5.893132398962174E-9</v>
+        <v>3.717918664460237E-10</v>
       </c>
       <c r="D4">
-        <v>6.2641304870262537E-10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.858565402867081E-09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>6.31860069401188E-8</v>
+        <v>6.283771202301914E-08</v>
       </c>
       <c r="C5">
-        <v>6.6857450585471627E-8</v>
+        <v>6.149710687622996E-08</v>
       </c>
       <c r="D5">
-        <v>6.2146582026061404E-8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.325347064040409E-08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>7.3613701340227354E-8</v>
+        <v>7.128281452242237E-08</v>
       </c>
       <c r="C6">
-        <v>7.8643715383395975E-8</v>
+        <v>6.224069060912201E-08</v>
       </c>
       <c r="D6">
-        <v>6.3399408123466654E-8</v>
+        <v>5.897060144613825E-08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>